<commit_message>
added test code for board-a proving that the clock, 3 analog inputs, daylight-savings time switch and msgeq7 and leds work
</commit_message>
<xml_diff>
--- a/New_Clock/Design Considerations and BoM.xlsx
+++ b/New_Clock/Design Considerations and BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huber\source\repos\infinity-mirror\New_Clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14290DF3-3CAF-49E4-A26E-65FBE0F931E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC7AF09-15CD-4585-95B7-6D3A7EE09B44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
   <si>
     <t>Quantity</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>8 SO</t>
+  </si>
+  <si>
+    <t>6 Pin Terminal Block</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -489,16 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -519,6 +513,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -852,24 +858,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -907,8 +913,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -931,8 +937,8 @@
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
     </row>
-    <row r="3" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+    <row r="3" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
@@ -961,8 +967,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="41"/>
       <c r="B4" s="29" t="s">
         <v>3</v>
       </c>
@@ -983,8 +989,8 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+    <row r="5" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
       <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
@@ -1003,8 +1009,8 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>84</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -1033,8 +1039,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
         <v>84</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1067,11 +1073,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -1099,8 +1105,8 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="40"/>
       <c r="B9" s="16" t="s">
         <v>7</v>
       </c>
@@ -1123,8 +1129,8 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+    <row r="10" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
       <c r="B10" s="16" t="s">
         <v>34</v>
       </c>
@@ -1145,8 +1151,8 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="40"/>
       <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
@@ -1173,8 +1179,8 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
       <c r="B12" s="16" t="s">
         <v>49</v>
       </c>
@@ -1203,8 +1209,8 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="40"/>
       <c r="B13" s="16" t="s">
         <v>60</v>
       </c>
@@ -1227,8 +1233,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="31"/>
       <c r="B14" s="23" t="s">
         <v>8</v>
       </c>
@@ -1245,8 +1251,8 @@
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
       <c r="B15" s="12" t="s">
         <v>9</v>
       </c>
@@ -1265,8 +1271,8 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13" t="s">
         <v>13</v>
@@ -1285,8 +1291,8 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="31"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="s">
         <v>14</v>
@@ -1303,8 +1309,8 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="30" t="s">
@@ -1325,8 +1331,8 @@
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -1357,8 +1363,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1368,7 +1374,7 @@
       <c r="D20" s="5">
         <v>1</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="34" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="5">
@@ -1388,8 +1394,8 @@
       </c>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="39"/>
       <c r="B21" s="16" t="s">
         <v>40</v>
       </c>
@@ -1416,8 +1422,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="39"/>
       <c r="B22" s="16" t="s">
         <v>52</v>
       </c>
@@ -1448,8 +1454,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="39"/>
       <c r="B23" s="16" t="s">
         <v>52</v>
       </c>
@@ -1480,8 +1486,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="39"/>
       <c r="B24" s="16" t="s">
         <v>52</v>
       </c>
@@ -1512,8 +1518,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="39"/>
       <c r="B25" s="16" t="s">
         <v>55</v>
       </c>
@@ -1523,7 +1529,7 @@
       <c r="D25" s="5">
         <v>1</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="34" t="s">
         <v>58</v>
       </c>
       <c r="F25" s="5">
@@ -1544,40 +1550,40 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="38" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="39"/>
+      <c r="B26" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="37">
         <v>1</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="37">
         <v>0.05</v>
       </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40" t="s">
+      <c r="G26" s="37"/>
+      <c r="H26" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="41" t="s">
+      <c r="I26" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="J26" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="J26" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
         <v>80</v>
       </c>
       <c r="B27" s="16" t="s">
@@ -1610,7 +1616,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" s="11"/>
     </row>
   </sheetData>
@@ -1647,14 +1658,14 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>37</v>
       </c>
@@ -1672,9 +1683,9 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:18" x14ac:dyDescent="0.3">
       <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1682,7 +1693,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:18" x14ac:dyDescent="0.3">
       <c r="J2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1693,22 +1704,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
       <c r="Q3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
       <c r="Q4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>28</v>
       </c>

</xml_diff>